<commit_message>
Additional detail to spreadsheet of files.
</commit_message>
<xml_diff>
--- a/docs/helcim-request-fields.xlsx
+++ b/docs/helcim-request-fields.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="166">
   <si>
     <t>Field Name</t>
   </si>
@@ -369,9 +369,6 @@
     <t>allowZeroAmount</t>
   </si>
   <si>
-    <t>1/numberic</t>
-  </si>
-  <si>
     <t>Allows a zero-dollar transaction to be processed so that a card-token can be generated.</t>
   </si>
   <si>
@@ -454,6 +451,69 @@
   </si>
   <si>
     <t>Either the date field or the search field must be provided, but not both.</t>
+  </si>
+  <si>
+    <t># Transaction History</t>
+  </si>
+  <si>
+    <t># Authentication</t>
+  </si>
+  <si>
+    <t># Card details</t>
+  </si>
+  <si>
+    <t># Tokenized car details</t>
+  </si>
+  <si>
+    <t># Amount</t>
+  </si>
+  <si>
+    <t># Past transaction reference</t>
+  </si>
+  <si>
+    <t># Address validation service</t>
+  </si>
+  <si>
+    <t># Recuring period details</t>
+  </si>
+  <si>
+    <t># Vendor metadata</t>
+  </si>
+  <si>
+    <t># Billing details</t>
+  </si>
+  <si>
+    <t># Shipping details</t>
+  </si>
+  <si>
+    <t># Amount details</t>
+  </si>
+  <si>
+    <t># Basket/cart content</t>
+  </si>
+  <si>
+    <t># Custom fields</t>
+  </si>
+  <si>
+    <t># Method</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>POST/GET</t>
+  </si>
+  <si>
+    <t># Endpoint path</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>/hosted</t>
+  </si>
+  <si>
+    <t>/api</t>
   </si>
 </sst>
 </file>
@@ -793,12 +853,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:O89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="900" topLeftCell="A46" activePane="bottomLeft"/>
+      <pane ySplit="900" activePane="bottomLeft"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A72" sqref="A72"/>
+      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +872,7 @@
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
     <col min="13" max="13" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.140625" customWidth="1"/>
   </cols>
@@ -825,19 +885,19 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" t="s">
         <v>131</v>
       </c>
-      <c r="E1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>132</v>
-      </c>
-      <c r="G1" t="s">
-        <v>133</v>
       </c>
       <c r="H1" t="s">
         <v>27</v>
@@ -852,7 +912,7 @@
         <v>48</v>
       </c>
       <c r="L1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M1" t="s">
         <v>31</v>
@@ -864,203 +924,193 @@
         <v>21</v>
       </c>
     </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" t="s">
+        <v>163</v>
+      </c>
+      <c r="J2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K2" t="s">
+        <v>163</v>
+      </c>
+      <c r="L2" t="s">
+        <v>165</v>
+      </c>
+      <c r="M2" t="s">
+        <v>93</v>
+      </c>
+    </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
+        <v>159</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>160</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>161</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>160</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>161</v>
       </c>
       <c r="H3" t="s">
-        <v>62</v>
+        <v>160</v>
       </c>
       <c r="I3" t="s">
-        <v>62</v>
+        <v>160</v>
       </c>
       <c r="J3" t="s">
-        <v>62</v>
+        <v>160</v>
       </c>
       <c r="K3" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="L3" t="s">
-        <v>62</v>
+        <v>161</v>
       </c>
       <c r="M3" t="s">
-        <v>62</v>
-      </c>
-      <c r="O3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E4" t="s">
-        <v>137</v>
-      </c>
-      <c r="F4" t="s">
-        <v>137</v>
-      </c>
-      <c r="G4" t="s">
-        <v>137</v>
-      </c>
-      <c r="H4" t="s">
-        <v>62</v>
-      </c>
-      <c r="I4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K4" t="s">
-        <v>62</v>
-      </c>
-      <c r="L4" t="s">
-        <v>62</v>
-      </c>
-      <c r="M4" t="s">
-        <v>62</v>
-      </c>
-      <c r="O4" t="s">
-        <v>6</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O5" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H6" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="I6" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="J6" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="K6" t="s">
-        <v>63</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
+      </c>
+      <c r="L6" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6" t="s">
+        <v>62</v>
       </c>
       <c r="O6" t="s">
-        <v>70</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F7" t="s">
+        <v>136</v>
+      </c>
+      <c r="G7" t="s">
+        <v>136</v>
+      </c>
+      <c r="H7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" t="s">
+        <v>62</v>
+      </c>
+      <c r="O7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>62</v>
+      </c>
+      <c r="I8" t="s">
+        <v>62</v>
       </c>
       <c r="J8" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="K8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>47</v>
@@ -1068,134 +1118,109 @@
       <c r="M8" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="N8" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="O8" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G9" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="H9" t="s">
-        <v>47</v>
+        <v>93</v>
+      </c>
+      <c r="I9" t="s">
+        <v>93</v>
       </c>
       <c r="J9" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="K9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>47</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>47</v>
+        <v>93</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="O9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K10" t="s">
-        <v>64</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O10" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
         <v>64</v>
       </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
         <v>64</v>
       </c>
-      <c r="G11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11" t="s">
-        <v>47</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" t="s">
         <v>64</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O11" t="s">
-        <v>20</v>
+      <c r="J12" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
         <v>64</v>
@@ -1212,6 +1237,9 @@
       <c r="H13" t="s">
         <v>47</v>
       </c>
+      <c r="I13" t="s">
+        <v>64</v>
+      </c>
       <c r="J13" t="s">
         <v>47</v>
       </c>
@@ -1225,15 +1253,15 @@
         <v>47</v>
       </c>
       <c r="O13" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
         <v>64</v>
@@ -1247,10 +1275,13 @@
       <c r="G14" t="s">
         <v>47</v>
       </c>
-      <c r="H14" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="H14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>47</v>
       </c>
       <c r="K14" t="s">
@@ -1262,241 +1293,198 @@
       <c r="M14" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="N14" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="O14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H16" t="s">
-        <v>62</v>
-      </c>
-      <c r="I16" t="s">
-        <v>62</v>
-      </c>
-      <c r="J16" t="s">
-        <v>93</v>
-      </c>
-      <c r="K16" t="s">
-        <v>62</v>
-      </c>
-      <c r="L16" t="s">
-        <v>47</v>
-      </c>
-      <c r="M16" t="s">
-        <v>47</v>
-      </c>
-      <c r="O16" t="s">
-        <v>10</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" t="s">
+        <v>64</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s">
         <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="G18" t="s">
         <v>47</v>
       </c>
       <c r="H18" t="s">
-        <v>62</v>
+        <v>47</v>
+      </c>
+      <c r="I18" t="s">
+        <v>64</v>
       </c>
       <c r="J18" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="K18" t="s">
-        <v>47</v>
-      </c>
-      <c r="L18" t="s">
+        <v>64</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M18" s="1" t="s">
         <v>47</v>
       </c>
       <c r="O18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" t="s">
-        <v>93</v>
-      </c>
-      <c r="H20" t="s">
-        <v>47</v>
-      </c>
-      <c r="I20" t="s">
-        <v>47</v>
-      </c>
-      <c r="K20" t="s">
-        <v>63</v>
-      </c>
-      <c r="L20" t="s">
-        <v>47</v>
-      </c>
-      <c r="M20" t="s">
-        <v>62</v>
-      </c>
-      <c r="O20" t="s">
-        <v>43</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" t="s">
+        <v>47</v>
+      </c>
+      <c r="I19" t="s">
+        <v>64</v>
+      </c>
+      <c r="J19" t="s">
+        <v>47</v>
+      </c>
+      <c r="K19" t="s">
+        <v>64</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" t="s">
-        <v>93</v>
-      </c>
-      <c r="H21" t="s">
-        <v>47</v>
-      </c>
-      <c r="I21" t="s">
-        <v>47</v>
-      </c>
-      <c r="K21" t="s">
-        <v>63</v>
-      </c>
-      <c r="L21" t="s">
-        <v>47</v>
-      </c>
-      <c r="M21" t="s">
-        <v>62</v>
-      </c>
-      <c r="O21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G23" t="s">
-        <v>47</v>
-      </c>
-      <c r="H23" t="s">
-        <v>47</v>
-      </c>
-      <c r="I23" t="s">
-        <v>47</v>
-      </c>
-      <c r="K23" t="s">
-        <v>62</v>
-      </c>
-      <c r="L23" t="s">
-        <v>47</v>
-      </c>
-      <c r="N23" t="s">
-        <v>60</v>
-      </c>
-      <c r="O23" t="s">
-        <v>51</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J22" t="s">
+        <v>62</v>
+      </c>
+      <c r="K22" t="s">
+        <v>62</v>
+      </c>
+      <c r="L22" t="s">
+        <v>47</v>
+      </c>
+      <c r="M22" t="s">
+        <v>47</v>
+      </c>
+      <c r="O22" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" t="s">
-        <v>47</v>
-      </c>
-      <c r="G24" t="s">
-        <v>47</v>
-      </c>
-      <c r="H24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I24" t="s">
-        <v>47</v>
-      </c>
-      <c r="K24" t="s">
-        <v>62</v>
-      </c>
-      <c r="L24" t="s">
-        <v>47</v>
-      </c>
-      <c r="O24" t="s">
-        <v>54</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
         <v>47</v>
@@ -1511,74 +1499,50 @@
         <v>47</v>
       </c>
       <c r="H25" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="I25" t="s">
-        <v>47</v>
+        <v>93</v>
+      </c>
+      <c r="J25" t="s">
+        <v>62</v>
       </c>
       <c r="K25" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="L25" t="s">
         <v>47</v>
       </c>
+      <c r="M25" t="s">
+        <v>47</v>
+      </c>
       <c r="O25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" t="s">
-        <v>47</v>
-      </c>
-      <c r="G26" t="s">
-        <v>47</v>
-      </c>
-      <c r="H26" t="s">
-        <v>47</v>
-      </c>
-      <c r="I26" t="s">
-        <v>47</v>
-      </c>
-      <c r="K26" t="s">
-        <v>62</v>
-      </c>
-      <c r="L26" t="s">
-        <v>47</v>
-      </c>
-      <c r="O26" t="s">
-        <v>59</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
         <v>63</v>
       </c>
       <c r="E28" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="F28" t="s">
         <v>63</v>
       </c>
       <c r="G28" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="H28" t="s">
         <v>47</v>
@@ -1586,19 +1550,25 @@
       <c r="I28" t="s">
         <v>47</v>
       </c>
+      <c r="J28" t="s">
+        <v>47</v>
+      </c>
       <c r="K28" t="s">
         <v>63</v>
       </c>
       <c r="L28" t="s">
         <v>47</v>
       </c>
+      <c r="M28" t="s">
+        <v>62</v>
+      </c>
       <c r="O28" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
         <v>45</v>
@@ -1607,13 +1577,13 @@
         <v>63</v>
       </c>
       <c r="E29" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="F29" t="s">
         <v>63</v>
       </c>
       <c r="G29" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="H29" t="s">
         <v>47</v>
@@ -1621,69 +1591,45 @@
       <c r="I29" t="s">
         <v>47</v>
       </c>
+      <c r="J29" t="s">
+        <v>47</v>
+      </c>
       <c r="K29" t="s">
         <v>63</v>
       </c>
       <c r="L29" t="s">
         <v>47</v>
       </c>
+      <c r="M29" t="s">
+        <v>62</v>
+      </c>
       <c r="O29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>110</v>
-      </c>
-      <c r="B30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" t="s">
-        <v>63</v>
-      </c>
-      <c r="F30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H30" t="s">
-        <v>47</v>
-      </c>
-      <c r="I30" t="s">
-        <v>47</v>
-      </c>
-      <c r="K30" t="s">
-        <v>47</v>
-      </c>
-      <c r="L30" t="s">
-        <v>47</v>
-      </c>
-      <c r="O30" t="s">
-        <v>111</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="D32" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="E32" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="F32" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G32" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="H32" t="s">
         <v>47</v>
@@ -1691,34 +1637,43 @@
       <c r="I32" t="s">
         <v>47</v>
       </c>
+      <c r="J32" t="s">
+        <v>47</v>
+      </c>
       <c r="K32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L32" t="s">
         <v>47</v>
       </c>
+      <c r="M32" t="s">
+        <v>47</v>
+      </c>
+      <c r="N32" t="s">
+        <v>60</v>
+      </c>
       <c r="O32" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D33" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="E33" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="F33" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G33" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="H33" t="s">
         <v>47</v>
@@ -1726,34 +1681,40 @@
       <c r="I33" t="s">
         <v>47</v>
       </c>
+      <c r="J33" t="s">
+        <v>47</v>
+      </c>
       <c r="K33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L33" t="s">
         <v>47</v>
       </c>
+      <c r="M33" t="s">
+        <v>47</v>
+      </c>
       <c r="O33" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="E34" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="F34" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G34" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="H34" t="s">
         <v>47</v>
@@ -1761,34 +1722,40 @@
       <c r="I34" t="s">
         <v>47</v>
       </c>
+      <c r="J34" t="s">
+        <v>47</v>
+      </c>
       <c r="K34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L34" t="s">
         <v>47</v>
       </c>
+      <c r="M34" t="s">
+        <v>47</v>
+      </c>
       <c r="O34" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D35" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="E35" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="F35" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G35" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="H35" t="s">
         <v>47</v>
@@ -1796,92 +1763,33 @@
       <c r="I35" t="s">
         <v>47</v>
       </c>
+      <c r="J35" t="s">
+        <v>47</v>
+      </c>
       <c r="K35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L35" t="s">
         <v>47</v>
       </c>
+      <c r="M35" t="s">
+        <v>47</v>
+      </c>
       <c r="O35" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>84</v>
-      </c>
-      <c r="B36" t="s">
-        <v>45</v>
-      </c>
-      <c r="D36" t="s">
-        <v>63</v>
-      </c>
-      <c r="E36" t="s">
-        <v>63</v>
-      </c>
-      <c r="F36" t="s">
-        <v>63</v>
-      </c>
-      <c r="G36" t="s">
-        <v>63</v>
-      </c>
-      <c r="H36" t="s">
-        <v>47</v>
-      </c>
-      <c r="I36" t="s">
-        <v>47</v>
-      </c>
-      <c r="K36" t="s">
-        <v>63</v>
-      </c>
-      <c r="L36" t="s">
-        <v>47</v>
-      </c>
-      <c r="O36" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>86</v>
-      </c>
-      <c r="B37" t="s">
-        <v>42</v>
-      </c>
-      <c r="D37" t="s">
-        <v>63</v>
-      </c>
-      <c r="E37" t="s">
-        <v>63</v>
-      </c>
-      <c r="F37" t="s">
-        <v>63</v>
-      </c>
-      <c r="G37" t="s">
-        <v>63</v>
-      </c>
-      <c r="H37" t="s">
-        <v>47</v>
-      </c>
-      <c r="I37" t="s">
-        <v>47</v>
-      </c>
-      <c r="K37" t="s">
-        <v>63</v>
-      </c>
-      <c r="L37" t="s">
-        <v>47</v>
-      </c>
-      <c r="O37" t="s">
-        <v>87</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D38" t="s">
         <v>63</v>
@@ -1907,16 +1815,19 @@
       <c r="L38" t="s">
         <v>47</v>
       </c>
+      <c r="M38" t="s">
+        <v>47</v>
+      </c>
       <c r="O38" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D39" t="s">
         <v>63</v>
@@ -1942,86 +1853,62 @@
       <c r="L39" t="s">
         <v>47</v>
       </c>
+      <c r="M39" t="s">
+        <v>47</v>
+      </c>
       <c r="O39" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>94</v>
-      </c>
-      <c r="B41" t="s">
-        <v>76</v>
-      </c>
-      <c r="D41" t="s">
-        <v>63</v>
-      </c>
-      <c r="E41" t="s">
-        <v>63</v>
-      </c>
-      <c r="F41" t="s">
-        <v>63</v>
-      </c>
-      <c r="G41" t="s">
-        <v>63</v>
-      </c>
-      <c r="H41" t="s">
-        <v>47</v>
-      </c>
-      <c r="I41" t="s">
-        <v>47</v>
-      </c>
-      <c r="K41" t="s">
-        <v>47</v>
-      </c>
-      <c r="L41" t="s">
-        <v>47</v>
-      </c>
-      <c r="O41" t="s">
-        <v>95</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" t="s">
+        <v>63</v>
+      </c>
+      <c r="F40" t="s">
+        <v>63</v>
+      </c>
+      <c r="G40" t="s">
+        <v>63</v>
+      </c>
+      <c r="H40" t="s">
+        <v>47</v>
+      </c>
+      <c r="I40" t="s">
+        <v>47</v>
+      </c>
+      <c r="K40" t="s">
+        <v>47</v>
+      </c>
+      <c r="L40" t="s">
+        <v>47</v>
+      </c>
+      <c r="M40" t="s">
+        <v>47</v>
+      </c>
+      <c r="O40" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>96</v>
-      </c>
-      <c r="B42" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" t="s">
-        <v>63</v>
-      </c>
-      <c r="E42" t="s">
-        <v>63</v>
-      </c>
-      <c r="F42" t="s">
-        <v>63</v>
-      </c>
-      <c r="G42" t="s">
-        <v>63</v>
-      </c>
-      <c r="H42" t="s">
-        <v>47</v>
-      </c>
-      <c r="I42" t="s">
-        <v>47</v>
-      </c>
-      <c r="K42" t="s">
-        <v>47</v>
-      </c>
-      <c r="L42" t="s">
-        <v>47</v>
-      </c>
-      <c r="O42" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="D43" t="s">
         <v>63</v>
@@ -2042,18 +1929,21 @@
         <v>47</v>
       </c>
       <c r="K43" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="L43" t="s">
         <v>47</v>
       </c>
+      <c r="M43" t="s">
+        <v>47</v>
+      </c>
       <c r="O43" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="B44" t="s">
         <v>42</v>
@@ -2077,21 +1967,24 @@
         <v>47</v>
       </c>
       <c r="K44" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="L44" t="s">
         <v>47</v>
       </c>
+      <c r="M44" t="s">
+        <v>47</v>
+      </c>
       <c r="O44" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D45" t="s">
         <v>63</v>
@@ -2112,18 +2005,21 @@
         <v>47</v>
       </c>
       <c r="K45" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="L45" t="s">
         <v>47</v>
       </c>
+      <c r="M45" t="s">
+        <v>47</v>
+      </c>
       <c r="O45" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="B46" t="s">
         <v>42</v>
@@ -2147,21 +2043,24 @@
         <v>47</v>
       </c>
       <c r="K46" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="L46" t="s">
         <v>47</v>
       </c>
+      <c r="M46" t="s">
+        <v>47</v>
+      </c>
       <c r="O46" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D47" t="s">
         <v>63</v>
@@ -2182,18 +2081,21 @@
         <v>47</v>
       </c>
       <c r="K47" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="L47" t="s">
         <v>47</v>
       </c>
+      <c r="M47" t="s">
+        <v>47</v>
+      </c>
       <c r="O47" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="B48" t="s">
         <v>42</v>
@@ -2217,21 +2119,62 @@
         <v>47</v>
       </c>
       <c r="K48" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="L48" t="s">
         <v>47</v>
       </c>
+      <c r="M48" t="s">
+        <v>47</v>
+      </c>
       <c r="O48" t="s">
-        <v>109</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49" t="s">
+        <v>63</v>
+      </c>
+      <c r="E49" t="s">
+        <v>63</v>
+      </c>
+      <c r="F49" t="s">
+        <v>63</v>
+      </c>
+      <c r="G49" t="s">
+        <v>63</v>
+      </c>
+      <c r="H49" t="s">
+        <v>47</v>
+      </c>
+      <c r="I49" t="s">
+        <v>47</v>
+      </c>
+      <c r="K49" t="s">
+        <v>63</v>
+      </c>
+      <c r="L49" t="s">
+        <v>47</v>
+      </c>
+      <c r="M49" t="s">
+        <v>47</v>
+      </c>
+      <c r="O49" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="D50" t="s">
         <v>63</v>
@@ -2252,91 +2195,67 @@
         <v>47</v>
       </c>
       <c r="K50" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="L50" t="s">
         <v>47</v>
       </c>
+      <c r="M50" t="s">
+        <v>47</v>
+      </c>
       <c r="O50" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>114</v>
-      </c>
-      <c r="B51" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" t="s">
-        <v>63</v>
-      </c>
-      <c r="E51" t="s">
-        <v>63</v>
-      </c>
-      <c r="F51" t="s">
-        <v>63</v>
-      </c>
-      <c r="G51" t="s">
-        <v>63</v>
-      </c>
-      <c r="H51" t="s">
-        <v>47</v>
-      </c>
-      <c r="I51" t="s">
-        <v>47</v>
-      </c>
-      <c r="K51" t="s">
-        <v>47</v>
-      </c>
-      <c r="L51" t="s">
-        <v>47</v>
-      </c>
-      <c r="O51" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>116</v>
-      </c>
-      <c r="B52" t="s">
-        <v>117</v>
-      </c>
-      <c r="D52" t="s">
-        <v>63</v>
-      </c>
-      <c r="E52" t="s">
-        <v>93</v>
-      </c>
-      <c r="F52" t="s">
-        <v>63</v>
-      </c>
-      <c r="G52" t="s">
-        <v>93</v>
-      </c>
-      <c r="H52" t="s">
-        <v>47</v>
-      </c>
-      <c r="I52" t="s">
-        <v>47</v>
-      </c>
-      <c r="K52" t="s">
-        <v>47</v>
-      </c>
-      <c r="L52" t="s">
-        <v>47</v>
-      </c>
-      <c r="O52" t="s">
-        <v>118</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" t="s">
+        <v>63</v>
+      </c>
+      <c r="E53" t="s">
+        <v>63</v>
+      </c>
+      <c r="F53" t="s">
+        <v>63</v>
+      </c>
+      <c r="G53" t="s">
+        <v>63</v>
+      </c>
+      <c r="H53" t="s">
+        <v>47</v>
+      </c>
+      <c r="I53" t="s">
+        <v>47</v>
+      </c>
+      <c r="K53" t="s">
+        <v>47</v>
+      </c>
+      <c r="L53" t="s">
+        <v>47</v>
+      </c>
+      <c r="M53" t="s">
+        <v>47</v>
+      </c>
+      <c r="O53" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="B54" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D54" t="s">
         <v>63</v>
@@ -2362,13 +2281,16 @@
       <c r="L54" t="s">
         <v>47</v>
       </c>
+      <c r="M54" t="s">
+        <v>47</v>
+      </c>
       <c r="O54" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="B55" t="s">
         <v>42</v>
@@ -2397,16 +2319,19 @@
       <c r="L55" t="s">
         <v>47</v>
       </c>
+      <c r="M55" t="s">
+        <v>47</v>
+      </c>
       <c r="O55" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="B56" t="s">
-        <v>125</v>
+        <v>42</v>
       </c>
       <c r="D56" t="s">
         <v>63</v>
@@ -2432,16 +2357,19 @@
       <c r="L56" t="s">
         <v>47</v>
       </c>
+      <c r="M56" t="s">
+        <v>47</v>
+      </c>
       <c r="O56" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="B57" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="D57" t="s">
         <v>63</v>
@@ -2467,16 +2395,19 @@
       <c r="L57" t="s">
         <v>47</v>
       </c>
+      <c r="M57" t="s">
+        <v>47</v>
+      </c>
       <c r="O57" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="B58" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="D58" t="s">
         <v>63</v>
@@ -2502,28 +2433,69 @@
       <c r="L58" t="s">
         <v>47</v>
       </c>
+      <c r="M58" t="s">
+        <v>47</v>
+      </c>
       <c r="O58" t="s">
-        <v>130</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" t="s">
+        <v>42</v>
+      </c>
+      <c r="D59" t="s">
+        <v>63</v>
+      </c>
+      <c r="E59" t="s">
+        <v>63</v>
+      </c>
+      <c r="F59" t="s">
+        <v>63</v>
+      </c>
+      <c r="G59" t="s">
+        <v>63</v>
+      </c>
+      <c r="H59" t="s">
+        <v>47</v>
+      </c>
+      <c r="I59" t="s">
+        <v>47</v>
+      </c>
+      <c r="K59" t="s">
+        <v>47</v>
+      </c>
+      <c r="L59" t="s">
+        <v>47</v>
+      </c>
+      <c r="M59" t="s">
+        <v>47</v>
+      </c>
+      <c r="O59" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="B60" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="D60" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="E60" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="F60" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="G60" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="H60" t="s">
         <v>47</v>
@@ -2535,132 +2507,503 @@
         <v>47</v>
       </c>
       <c r="L60" t="s">
-        <v>144</v>
+        <v>47</v>
+      </c>
+      <c r="M60" t="s">
+        <v>47</v>
       </c>
       <c r="O60" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>30</v>
-      </c>
-      <c r="B61" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" t="s">
-        <v>47</v>
-      </c>
-      <c r="E61" t="s">
-        <v>47</v>
-      </c>
-      <c r="F61" t="s">
-        <v>47</v>
-      </c>
-      <c r="G61" t="s">
-        <v>47</v>
-      </c>
-      <c r="H61" t="s">
-        <v>47</v>
-      </c>
-      <c r="I61" t="s">
-        <v>47</v>
-      </c>
-      <c r="K61" t="s">
-        <v>47</v>
-      </c>
-      <c r="L61" t="s">
-        <v>144</v>
-      </c>
-      <c r="O61" t="s">
-        <v>143</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>112</v>
+      </c>
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" t="s">
+        <v>63</v>
+      </c>
+      <c r="E63" t="s">
+        <v>63</v>
+      </c>
+      <c r="F63" t="s">
+        <v>63</v>
+      </c>
+      <c r="G63" t="s">
+        <v>63</v>
+      </c>
+      <c r="H63" t="s">
+        <v>47</v>
+      </c>
+      <c r="I63" t="s">
+        <v>47</v>
+      </c>
+      <c r="K63" t="s">
+        <v>47</v>
+      </c>
+      <c r="L63" t="s">
+        <v>47</v>
+      </c>
+      <c r="M63" t="s">
+        <v>47</v>
+      </c>
+      <c r="O63" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>114</v>
+      </c>
+      <c r="B64" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" t="s">
+        <v>63</v>
+      </c>
+      <c r="E64" t="s">
+        <v>63</v>
+      </c>
+      <c r="F64" t="s">
+        <v>63</v>
+      </c>
+      <c r="G64" t="s">
+        <v>63</v>
+      </c>
+      <c r="H64" t="s">
+        <v>47</v>
+      </c>
+      <c r="I64" t="s">
+        <v>47</v>
+      </c>
+      <c r="K64" t="s">
+        <v>47</v>
+      </c>
+      <c r="L64" t="s">
+        <v>47</v>
+      </c>
+      <c r="M64" t="s">
+        <v>47</v>
+      </c>
+      <c r="O64" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>116</v>
+      </c>
+      <c r="B65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" t="s">
+        <v>63</v>
+      </c>
+      <c r="E65" t="s">
+        <v>93</v>
+      </c>
+      <c r="F65" t="s">
+        <v>63</v>
+      </c>
+      <c r="G65" t="s">
+        <v>93</v>
+      </c>
+      <c r="H65" t="s">
+        <v>47</v>
+      </c>
+      <c r="I65" t="s">
+        <v>47</v>
+      </c>
+      <c r="K65" t="s">
+        <v>47</v>
+      </c>
+      <c r="L65" t="s">
+        <v>47</v>
+      </c>
+      <c r="M65" t="s">
+        <v>47</v>
+      </c>
+      <c r="O65" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>119</v>
+      </c>
+      <c r="B68" t="s">
+        <v>45</v>
+      </c>
+      <c r="D68" t="s">
+        <v>63</v>
+      </c>
+      <c r="E68" t="s">
+        <v>63</v>
+      </c>
+      <c r="F68" t="s">
+        <v>63</v>
+      </c>
+      <c r="G68" t="s">
+        <v>63</v>
+      </c>
+      <c r="H68" t="s">
+        <v>47</v>
+      </c>
+      <c r="I68" t="s">
+        <v>47</v>
+      </c>
+      <c r="K68" t="s">
+        <v>47</v>
+      </c>
+      <c r="L68" t="s">
+        <v>47</v>
+      </c>
+      <c r="M68" t="s">
+        <v>47</v>
+      </c>
+      <c r="O68" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>121</v>
+      </c>
+      <c r="B69" t="s">
+        <v>42</v>
+      </c>
+      <c r="D69" t="s">
+        <v>63</v>
+      </c>
+      <c r="E69" t="s">
+        <v>63</v>
+      </c>
+      <c r="F69" t="s">
+        <v>63</v>
+      </c>
+      <c r="G69" t="s">
+        <v>63</v>
+      </c>
+      <c r="H69" t="s">
+        <v>47</v>
+      </c>
+      <c r="I69" t="s">
+        <v>47</v>
+      </c>
+      <c r="K69" t="s">
+        <v>47</v>
+      </c>
+      <c r="L69" t="s">
+        <v>47</v>
+      </c>
+      <c r="M69" t="s">
+        <v>47</v>
+      </c>
+      <c r="O69" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>123</v>
+      </c>
+      <c r="B70" t="s">
+        <v>124</v>
+      </c>
+      <c r="D70" t="s">
+        <v>63</v>
+      </c>
+      <c r="E70" t="s">
+        <v>63</v>
+      </c>
+      <c r="F70" t="s">
+        <v>63</v>
+      </c>
+      <c r="G70" t="s">
+        <v>63</v>
+      </c>
+      <c r="H70" t="s">
+        <v>47</v>
+      </c>
+      <c r="I70" t="s">
+        <v>47</v>
+      </c>
+      <c r="K70" t="s">
+        <v>47</v>
+      </c>
+      <c r="L70" t="s">
+        <v>47</v>
+      </c>
+      <c r="M70" t="s">
+        <v>47</v>
+      </c>
+      <c r="O70" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>126</v>
+      </c>
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71" t="s">
+        <v>63</v>
+      </c>
+      <c r="E71" t="s">
+        <v>63</v>
+      </c>
+      <c r="F71" t="s">
+        <v>63</v>
+      </c>
+      <c r="G71" t="s">
+        <v>63</v>
+      </c>
+      <c r="H71" t="s">
+        <v>47</v>
+      </c>
+      <c r="I71" t="s">
+        <v>47</v>
+      </c>
+      <c r="K71" t="s">
+        <v>47</v>
+      </c>
+      <c r="L71" t="s">
+        <v>47</v>
+      </c>
+      <c r="M71" t="s">
+        <v>47</v>
+      </c>
+      <c r="O71" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>128</v>
+      </c>
+      <c r="B72" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72" t="s">
+        <v>63</v>
+      </c>
+      <c r="E72" t="s">
+        <v>63</v>
+      </c>
+      <c r="F72" t="s">
+        <v>63</v>
+      </c>
+      <c r="G72" t="s">
+        <v>63</v>
+      </c>
+      <c r="H72" t="s">
+        <v>47</v>
+      </c>
+      <c r="I72" t="s">
+        <v>47</v>
+      </c>
+      <c r="K72" t="s">
+        <v>47</v>
+      </c>
+      <c r="L72" t="s">
+        <v>47</v>
+      </c>
+      <c r="M72" t="s">
+        <v>47</v>
+      </c>
+      <c r="O72" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>139</v>
+      </c>
+      <c r="B75" t="s">
+        <v>140</v>
+      </c>
+      <c r="D75" t="s">
+        <v>47</v>
+      </c>
+      <c r="E75" t="s">
+        <v>47</v>
+      </c>
+      <c r="F75" t="s">
+        <v>47</v>
+      </c>
+      <c r="G75" t="s">
+        <v>47</v>
+      </c>
+      <c r="H75" t="s">
+        <v>47</v>
+      </c>
+      <c r="I75" t="s">
+        <v>47</v>
+      </c>
+      <c r="K75" t="s">
+        <v>47</v>
+      </c>
+      <c r="L75" t="s">
+        <v>143</v>
+      </c>
+      <c r="M75" t="s">
+        <v>47</v>
+      </c>
+      <c r="O75" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>30</v>
+      </c>
+      <c r="B76" t="s">
+        <v>5</v>
+      </c>
+      <c r="D76" t="s">
+        <v>47</v>
+      </c>
+      <c r="E76" t="s">
+        <v>47</v>
+      </c>
+      <c r="F76" t="s">
+        <v>47</v>
+      </c>
+      <c r="G76" t="s">
+        <v>47</v>
+      </c>
+      <c r="H76" t="s">
+        <v>47</v>
+      </c>
+      <c r="I76" t="s">
+        <v>47</v>
+      </c>
+      <c r="K76" t="s">
+        <v>47</v>
+      </c>
+      <c r="L76" t="s">
+        <v>143</v>
+      </c>
+      <c r="M76" t="s">
+        <v>47</v>
+      </c>
+      <c r="O76" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>135</v>
+      </c>
+      <c r="D79" t="s">
+        <v>47</v>
+      </c>
+      <c r="E79" t="s">
+        <v>63</v>
+      </c>
+      <c r="F79" t="s">
+        <v>47</v>
+      </c>
+      <c r="G79" t="s">
+        <v>63</v>
+      </c>
+      <c r="H79" t="s">
+        <v>47</v>
+      </c>
+      <c r="I79" t="s">
+        <v>47</v>
+      </c>
+      <c r="K79" t="s">
+        <v>47</v>
+      </c>
+      <c r="L79" t="s">
+        <v>47</v>
+      </c>
+      <c r="M79" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>62</v>
+      </c>
+      <c r="B82" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>63</v>
+      </c>
+      <c r="B83" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>47</v>
+      </c>
+      <c r="B84" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>64</v>
+      </c>
+      <c r="B85" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>136</v>
       </c>
-      <c r="D63" t="s">
-        <v>47</v>
-      </c>
-      <c r="E63" t="s">
-        <v>63</v>
-      </c>
-      <c r="F63" t="s">
-        <v>47</v>
-      </c>
-      <c r="G63" t="s">
-        <v>63</v>
-      </c>
-      <c r="H63" t="s">
-        <v>47</v>
-      </c>
-      <c r="I63" t="s">
-        <v>47</v>
-      </c>
-      <c r="K63" t="s">
-        <v>47</v>
-      </c>
-      <c r="L63" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>62</v>
-      </c>
-      <c r="B66" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>63</v>
-      </c>
-      <c r="B67" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>47</v>
-      </c>
-      <c r="B68" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>64</v>
-      </c>
-      <c r="B69" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="B86" t="s">
         <v>137</v>
       </c>
-      <c r="B70" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>143</v>
+      </c>
+      <c r="B87" t="s">
         <v>144</v>
       </c>
-      <c r="B71" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>119</v>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>